<commit_message>
Endurance ISSM Cal sheets
added missing serial number for MOPAK
</commit_message>
<xml_diff>
--- a/CE01ISSM/Omaha_Cal_Info_CE01ISSM_00004.xlsx
+++ b/CE01ISSM/Omaha_Cal_Info_CE01ISSM_00004.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="781" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="782" uniqueCount="185">
   <si>
     <t>Ref Des</t>
   </si>
@@ -416,43 +416,22 @@
     <t>CE01ISSM-SBC11-00-CPMENG000</t>
   </si>
   <si>
-    <t>CP03ISSM-00002-CPM1</t>
-  </si>
-  <si>
     <t>CE01ISSM-RIC21-00-CPMENG000</t>
-  </si>
-  <si>
-    <t>CP03ISSM-00002-CPM2</t>
   </si>
   <si>
     <t>CE01ISSM-MFC31-00-CPMENG000</t>
   </si>
   <si>
-    <t>CP03ISSM-00002-CPM3</t>
-  </si>
-  <si>
     <t>CE01ISSM-SBD17-00-DCLENG000</t>
-  </si>
-  <si>
-    <t>CP03ISSM-00002-DCL17</t>
   </si>
   <si>
     <t>CE01ISSM-RID16-00-DCLENG000</t>
   </si>
   <si>
-    <t>CP03ISSM-00002-DCL16</t>
-  </si>
-  <si>
     <t>CE01ISSM-MFD35-00-DCLENG000</t>
   </si>
   <si>
-    <t>CP03ISSM-00002-DCL35</t>
-  </si>
-  <si>
     <t>CE01ISSM-MFD37-00-DCLENG000</t>
-  </si>
-  <si>
-    <t>CP03ISSM-00002-DCL37</t>
   </si>
   <si>
     <t>CE01ISSM-00004</t>
@@ -602,6 +581,27 @@
   </si>
   <si>
     <t>CE01ISSM-MFD37-07-ZPLSCC000</t>
+  </si>
+  <si>
+    <t>CE01ISSM-MOPAK</t>
+  </si>
+  <si>
+    <t>CE01ISSM-SBC11ENG</t>
+  </si>
+  <si>
+    <t>CE01ISSM-MFC31ENG</t>
+  </si>
+  <si>
+    <t>CE01ISSM-SBD17ENG</t>
+  </si>
+  <si>
+    <t>CE01ISSM-RID16ENG</t>
+  </si>
+  <si>
+    <t>CE01ISSM-MFD35ENG</t>
+  </si>
+  <si>
+    <t>CE01ISSM-MFD37ENG</t>
   </si>
 </sst>
 </file>
@@ -1883,10 +1883,10 @@
         <v>10</v>
       </c>
       <c r="L1" s="54" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="M1" s="54" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -1894,7 +1894,7 @@
         <v>11</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C2" s="12">
         <v>4</v>
@@ -1907,16 +1907,16 @@
       </c>
       <c r="F2" s="49"/>
       <c r="G2" s="51" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="H2" s="51" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="I2" s="52">
         <v>25</v>
       </c>
       <c r="J2" s="51" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="K2" s="53"/>
       <c r="L2" s="60">
@@ -1936,8 +1936,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK226"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" topLeftCell="A211" workbookViewId="0">
+      <selection activeCell="C230" sqref="C230"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3009,13 +3009,13 @@
         <v>54</v>
       </c>
       <c r="H3" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="I3" s="13">
         <v>4</v>
       </c>
       <c r="J3" s="22" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="K3" s="16" t="s">
         <v>19</v>
@@ -3030,13 +3030,13 @@
         <v>54</v>
       </c>
       <c r="H4" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="I4" s="13">
         <v>4</v>
       </c>
       <c r="J4" s="22" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="K4" s="16" t="s">
         <v>20</v>
@@ -3051,13 +3051,13 @@
         <v>54</v>
       </c>
       <c r="H5" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="I5" s="13">
         <v>4</v>
       </c>
       <c r="J5" s="22" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="K5" s="16" t="s">
         <v>56</v>
@@ -3072,13 +3072,13 @@
         <v>54</v>
       </c>
       <c r="H6" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="I6" s="13">
         <v>4</v>
       </c>
       <c r="J6" s="22" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="K6" s="16" t="s">
         <v>57</v>
@@ -3093,13 +3093,13 @@
         <v>54</v>
       </c>
       <c r="H7" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="I7" s="13">
         <v>4</v>
       </c>
       <c r="J7" s="22" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="K7" s="16" t="s">
         <v>58</v>
@@ -3114,13 +3114,13 @@
         <v>54</v>
       </c>
       <c r="H8" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="I8" s="13">
         <v>4</v>
       </c>
       <c r="J8" s="22" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="K8" s="16" t="s">
         <v>59</v>
@@ -3135,13 +3135,13 @@
         <v>54</v>
       </c>
       <c r="H9" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="I9" s="13">
         <v>4</v>
       </c>
       <c r="J9" s="22" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="K9" s="16" t="s">
         <v>60</v>
@@ -3156,13 +3156,13 @@
         <v>54</v>
       </c>
       <c r="H10" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="I10" s="13">
         <v>4</v>
       </c>
       <c r="J10" s="22" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="K10" s="16" t="s">
         <v>61</v>
@@ -3177,13 +3177,13 @@
         <v>54</v>
       </c>
       <c r="H11" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="I11" s="13">
         <v>4</v>
       </c>
       <c r="J11" s="22" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="K11" s="16" t="s">
         <v>62</v>
@@ -3198,13 +3198,13 @@
         <v>54</v>
       </c>
       <c r="H12" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="I12" s="13">
         <v>4</v>
       </c>
       <c r="J12" s="22" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="K12" s="16" t="s">
         <v>63</v>
@@ -3219,13 +3219,13 @@
         <v>54</v>
       </c>
       <c r="H13" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="I13" s="13">
         <v>4</v>
       </c>
       <c r="J13" s="22" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="K13" s="16" t="s">
         <v>64</v>
@@ -3240,13 +3240,13 @@
         <v>54</v>
       </c>
       <c r="H14" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="I14" s="13">
         <v>4</v>
       </c>
       <c r="J14" s="22" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="K14" s="16" t="s">
         <v>65</v>
@@ -3261,13 +3261,13 @@
         <v>54</v>
       </c>
       <c r="H15" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="I15" s="13">
         <v>4</v>
       </c>
       <c r="J15" s="22" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="K15" s="16" t="s">
         <v>66</v>
@@ -3282,13 +3282,13 @@
         <v>54</v>
       </c>
       <c r="H16" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="I16" s="13">
         <v>4</v>
       </c>
       <c r="J16" s="22" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="K16" s="16" t="s">
         <v>67</v>
@@ -3303,13 +3303,13 @@
         <v>54</v>
       </c>
       <c r="H17" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="I17" s="13">
         <v>4</v>
       </c>
       <c r="J17" s="22" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="K17" s="16" t="s">
         <v>68</v>
@@ -3324,13 +3324,13 @@
         <v>54</v>
       </c>
       <c r="H18" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="I18" s="13">
         <v>4</v>
       </c>
       <c r="J18" s="22" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="K18" s="16" t="s">
         <v>69</v>
@@ -3345,13 +3345,13 @@
         <v>54</v>
       </c>
       <c r="H19" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="I19" s="13">
         <v>4</v>
       </c>
       <c r="J19" s="22" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="K19" s="16" t="s">
         <v>70</v>
@@ -3366,13 +3366,13 @@
         <v>54</v>
       </c>
       <c r="H20" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="I20" s="13">
         <v>4</v>
       </c>
       <c r="J20" s="22" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="K20" s="16" t="s">
         <v>71</v>
@@ -3387,13 +3387,13 @@
         <v>54</v>
       </c>
       <c r="H21" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="I21" s="13">
         <v>4</v>
       </c>
       <c r="J21" s="22" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="K21" s="16" t="s">
         <v>72</v>
@@ -3408,13 +3408,13 @@
         <v>54</v>
       </c>
       <c r="H22" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="I22" s="13">
         <v>4</v>
       </c>
       <c r="J22" s="22" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="K22" s="16" t="s">
         <v>73</v>
@@ -3429,13 +3429,13 @@
         <v>54</v>
       </c>
       <c r="H23" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="I23" s="13">
         <v>4</v>
       </c>
       <c r="J23" s="22" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="K23" s="16" t="s">
         <v>74</v>
@@ -3450,13 +3450,13 @@
         <v>54</v>
       </c>
       <c r="H24" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="I24" s="13">
         <v>4</v>
       </c>
       <c r="J24" s="22" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="K24" s="16" t="s">
         <v>75</v>
@@ -3471,13 +3471,13 @@
         <v>54</v>
       </c>
       <c r="H25" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="I25" s="13">
         <v>4</v>
       </c>
       <c r="J25" s="22" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="K25" s="16" t="s">
         <v>76</v>
@@ -3492,13 +3492,13 @@
         <v>54</v>
       </c>
       <c r="H26" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="I26" s="13">
         <v>4</v>
       </c>
       <c r="J26" s="22" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="K26" s="16" t="s">
         <v>77</v>
@@ -3522,7 +3522,7 @@
         <v>42</v>
       </c>
       <c r="H28" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="I28" s="13">
         <v>4</v>
@@ -3543,7 +3543,7 @@
         <v>42</v>
       </c>
       <c r="H29" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="I29" s="13">
         <v>4</v>
@@ -3564,7 +3564,7 @@
         <v>42</v>
       </c>
       <c r="H30" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="I30" s="13">
         <v>4</v>
@@ -3585,7 +3585,7 @@
         <v>42</v>
       </c>
       <c r="H31" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="I31" s="13">
         <v>4</v>
@@ -3606,7 +3606,7 @@
         <v>42</v>
       </c>
       <c r="H32" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="I32" s="13">
         <v>4</v>
@@ -3627,7 +3627,7 @@
         <v>42</v>
       </c>
       <c r="H33" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="I33" s="13">
         <v>4</v>
@@ -3648,7 +3648,7 @@
         <v>42</v>
       </c>
       <c r="H34" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="I34" s="13">
         <v>4</v>
@@ -3663,7 +3663,7 @@
         <v>124</v>
       </c>
       <c r="M34" s="13" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
     </row>
     <row r="35" spans="1:1024" x14ac:dyDescent="0.25">
@@ -3671,7 +3671,7 @@
         <v>42</v>
       </c>
       <c r="H35" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="I35" s="13">
         <v>4</v>
@@ -3694,7 +3694,7 @@
         <v>42</v>
       </c>
       <c r="H36" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="I36" s="13">
         <v>4</v>
@@ -3709,7 +3709,7 @@
         <v>1.0760000000000001</v>
       </c>
       <c r="M36" s="13" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
     </row>
     <row r="37" spans="1:1024" x14ac:dyDescent="0.25">
@@ -3717,7 +3717,7 @@
         <v>42</v>
       </c>
       <c r="H37" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="I37" s="13">
         <v>4</v>
@@ -3749,12 +3749,14 @@
         <v>16</v>
       </c>
       <c r="B39" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C39" s="13">
         <v>4</v>
       </c>
-      <c r="D39" s="43"/>
+      <c r="D39" s="19" t="s">
+        <v>178</v>
+      </c>
       <c r="E39" s="16"/>
       <c r="F39" s="36"/>
       <c r="G39" s="13" t="s">
@@ -5807,7 +5809,7 @@
         <v>18</v>
       </c>
       <c r="B41" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C41" s="13">
         <v>4</v>
@@ -6844,7 +6846,7 @@
         <v>18</v>
       </c>
       <c r="B42" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C42" s="13">
         <v>4</v>
@@ -8906,13 +8908,13 @@
         <v>55</v>
       </c>
       <c r="B44" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C44" s="13">
         <v>4</v>
       </c>
       <c r="D44" s="22" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="E44" s="16" t="s">
         <v>19</v>
@@ -8927,13 +8929,13 @@
         <v>55</v>
       </c>
       <c r="B45" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C45" s="13">
         <v>4</v>
       </c>
       <c r="D45" s="22" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="E45" s="16" t="s">
         <v>20</v>
@@ -8948,13 +8950,13 @@
         <v>55</v>
       </c>
       <c r="B46" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C46" s="13">
         <v>4</v>
       </c>
       <c r="D46" s="22" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="E46" s="16" t="s">
         <v>56</v>
@@ -8969,13 +8971,13 @@
         <v>55</v>
       </c>
       <c r="B47" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C47" s="13">
         <v>4</v>
       </c>
       <c r="D47" s="22" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="E47" s="16" t="s">
         <v>57</v>
@@ -8990,13 +8992,13 @@
         <v>55</v>
       </c>
       <c r="B48" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C48" s="13">
         <v>4</v>
       </c>
       <c r="D48" s="22" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="E48" s="16" t="s">
         <v>58</v>
@@ -9011,13 +9013,13 @@
         <v>55</v>
       </c>
       <c r="B49" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C49" s="13">
         <v>4</v>
       </c>
       <c r="D49" s="22" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="E49" s="16" t="s">
         <v>59</v>
@@ -9032,13 +9034,13 @@
         <v>55</v>
       </c>
       <c r="B50" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C50" s="13">
         <v>4</v>
       </c>
       <c r="D50" s="22" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="E50" s="16" t="s">
         <v>60</v>
@@ -9053,13 +9055,13 @@
         <v>55</v>
       </c>
       <c r="B51" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C51" s="13">
         <v>4</v>
       </c>
       <c r="D51" s="22" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="E51" s="16" t="s">
         <v>61</v>
@@ -9074,13 +9076,13 @@
         <v>55</v>
       </c>
       <c r="B52" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C52" s="13">
         <v>4</v>
       </c>
       <c r="D52" s="22" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="E52" s="16" t="s">
         <v>62</v>
@@ -9095,13 +9097,13 @@
         <v>55</v>
       </c>
       <c r="B53" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C53" s="13">
         <v>4</v>
       </c>
       <c r="D53" s="22" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="E53" s="16" t="s">
         <v>63</v>
@@ -9116,13 +9118,13 @@
         <v>55</v>
       </c>
       <c r="B54" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C54" s="13">
         <v>4</v>
       </c>
       <c r="D54" s="22" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="E54" s="16" t="s">
         <v>64</v>
@@ -9137,13 +9139,13 @@
         <v>55</v>
       </c>
       <c r="B55" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C55" s="13">
         <v>4</v>
       </c>
       <c r="D55" s="22" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="E55" s="16" t="s">
         <v>65</v>
@@ -9158,13 +9160,13 @@
         <v>55</v>
       </c>
       <c r="B56" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C56" s="13">
         <v>4</v>
       </c>
       <c r="D56" s="22" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="E56" s="16" t="s">
         <v>66</v>
@@ -9179,13 +9181,13 @@
         <v>55</v>
       </c>
       <c r="B57" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C57" s="13">
         <v>4</v>
       </c>
       <c r="D57" s="22" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="E57" s="16" t="s">
         <v>67</v>
@@ -9200,13 +9202,13 @@
         <v>55</v>
       </c>
       <c r="B58" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C58" s="13">
         <v>4</v>
       </c>
       <c r="D58" s="22" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="E58" s="16" t="s">
         <v>68</v>
@@ -9221,13 +9223,13 @@
         <v>55</v>
       </c>
       <c r="B59" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C59" s="13">
         <v>4</v>
       </c>
       <c r="D59" s="22" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="E59" s="16" t="s">
         <v>69</v>
@@ -9242,13 +9244,13 @@
         <v>55</v>
       </c>
       <c r="B60" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C60" s="13">
         <v>4</v>
       </c>
       <c r="D60" s="22" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="E60" s="16" t="s">
         <v>70</v>
@@ -9263,13 +9265,13 @@
         <v>55</v>
       </c>
       <c r="B61" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C61" s="13">
         <v>4</v>
       </c>
       <c r="D61" s="22" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="E61" s="16" t="s">
         <v>71</v>
@@ -9284,13 +9286,13 @@
         <v>55</v>
       </c>
       <c r="B62" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C62" s="13">
         <v>4</v>
       </c>
       <c r="D62" s="22" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="E62" s="16" t="s">
         <v>72</v>
@@ -9305,13 +9307,13 @@
         <v>55</v>
       </c>
       <c r="B63" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C63" s="13">
         <v>4</v>
       </c>
       <c r="D63" s="22" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="E63" s="16" t="s">
         <v>73</v>
@@ -9326,13 +9328,13 @@
         <v>55</v>
       </c>
       <c r="B64" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C64" s="13">
         <v>4</v>
       </c>
       <c r="D64" s="22" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="E64" s="16" t="s">
         <v>74</v>
@@ -9347,13 +9349,13 @@
         <v>55</v>
       </c>
       <c r="B65" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C65" s="13">
         <v>4</v>
       </c>
       <c r="D65" s="22" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="E65" s="16" t="s">
         <v>75</v>
@@ -9368,13 +9370,13 @@
         <v>55</v>
       </c>
       <c r="B66" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C66" s="13">
         <v>4</v>
       </c>
       <c r="D66" s="22" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="E66" s="16" t="s">
         <v>76</v>
@@ -9389,13 +9391,13 @@
         <v>55</v>
       </c>
       <c r="B67" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C67" s="13">
         <v>4</v>
       </c>
       <c r="D67" s="22" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="E67" s="16" t="s">
         <v>77</v>
@@ -9419,7 +9421,7 @@
         <v>79</v>
       </c>
       <c r="B69" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C69" s="13">
         <v>4</v>
@@ -9440,7 +9442,7 @@
         <v>79</v>
       </c>
       <c r="B70" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C70" s="13">
         <v>4</v>
@@ -9461,7 +9463,7 @@
         <v>79</v>
       </c>
       <c r="B71" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C71" s="13">
         <v>4</v>
@@ -9473,7 +9475,7 @@
         <v>80</v>
       </c>
       <c r="F71" s="39" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="G71"/>
     </row>
@@ -9482,7 +9484,7 @@
         <v>79</v>
       </c>
       <c r="B72" s="16" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C72" s="16">
         <v>4</v>
@@ -9491,13 +9493,13 @@
         <v>477</v>
       </c>
       <c r="E72" s="32" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="F72" s="33" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="G72" s="32" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="H72" s="16"/>
       <c r="I72" s="16"/>
@@ -10532,7 +10534,7 @@
         <v>53</v>
       </c>
       <c r="B74" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C74" s="13">
         <v>4</v>
@@ -10553,7 +10555,7 @@
         <v>53</v>
       </c>
       <c r="B75" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C75" s="13">
         <v>4</v>
@@ -10574,7 +10576,7 @@
         <v>53</v>
       </c>
       <c r="B76" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C76" s="13">
         <v>4</v>
@@ -10595,7 +10597,7 @@
         <v>53</v>
       </c>
       <c r="B77" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C77" s="13">
         <v>4</v>
@@ -10616,7 +10618,7 @@
         <v>53</v>
       </c>
       <c r="B78" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C78" s="13">
         <v>4</v>
@@ -10637,7 +10639,7 @@
         <v>53</v>
       </c>
       <c r="B79" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C79" s="13">
         <v>4</v>
@@ -10658,7 +10660,7 @@
         <v>53</v>
       </c>
       <c r="B80" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C80" s="13">
         <v>4</v>
@@ -10673,7 +10675,7 @@
         <v>124</v>
       </c>
       <c r="G80" s="16" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
     </row>
     <row r="81" spans="1:1024" x14ac:dyDescent="0.25">
@@ -10681,7 +10683,7 @@
         <v>53</v>
       </c>
       <c r="B81" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C81" s="13">
         <v>4</v>
@@ -10704,7 +10706,7 @@
         <v>53</v>
       </c>
       <c r="B82" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C82" s="13">
         <v>4</v>
@@ -10719,7 +10721,7 @@
         <v>1.0760000000000001</v>
       </c>
       <c r="G82" s="16" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
     </row>
     <row r="83" spans="1:1024" x14ac:dyDescent="0.25">
@@ -10727,7 +10729,7 @@
         <v>53</v>
       </c>
       <c r="B83" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C83" s="13">
         <v>4</v>
@@ -10759,7 +10761,7 @@
         <v>82</v>
       </c>
       <c r="B85" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C85" s="13">
         <v>4</v>
@@ -10782,7 +10784,7 @@
         <v>82</v>
       </c>
       <c r="B86" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C86" s="13">
         <v>4</v>
@@ -10805,7 +10807,7 @@
         <v>82</v>
       </c>
       <c r="B87" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C87" s="13">
         <v>4</v>
@@ -10826,7 +10828,7 @@
         <v>82</v>
       </c>
       <c r="B88" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C88" s="13">
         <v>4</v>
@@ -10838,7 +10840,7 @@
         <v>86</v>
       </c>
       <c r="F88" s="42" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="G88"/>
     </row>
@@ -10847,7 +10849,7 @@
         <v>82</v>
       </c>
       <c r="B89" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C89" s="13">
         <v>4</v>
@@ -10859,7 +10861,7 @@
         <v>87</v>
       </c>
       <c r="F89" s="42" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="G89"/>
     </row>
@@ -10868,7 +10870,7 @@
         <v>82</v>
       </c>
       <c r="B90" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C90" s="13">
         <v>4</v>
@@ -10880,7 +10882,7 @@
         <v>88</v>
       </c>
       <c r="F90" s="42" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="G90"/>
     </row>
@@ -10889,7 +10891,7 @@
         <v>82</v>
       </c>
       <c r="B91" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C91" s="13">
         <v>4</v>
@@ -10901,7 +10903,7 @@
         <v>89</v>
       </c>
       <c r="F91" s="42" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="G91"/>
     </row>
@@ -10919,7 +10921,7 @@
         <v>32</v>
       </c>
       <c r="B93" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C93" s="13">
         <v>4</v>
@@ -10931,7 +10933,7 @@
         <v>33</v>
       </c>
       <c r="F93" s="58" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="G93"/>
       <c r="H93"/>
@@ -11956,7 +11958,7 @@
         <v>32</v>
       </c>
       <c r="B94" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C94" s="13">
         <v>4</v>
@@ -11968,7 +11970,7 @@
         <v>34</v>
       </c>
       <c r="F94" s="58" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="G94"/>
       <c r="H94"/>
@@ -12994,7 +12996,7 @@
         <v>32</v>
       </c>
       <c r="B95" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C95" s="13">
         <v>4</v>
@@ -14032,7 +14034,7 @@
         <v>32</v>
       </c>
       <c r="B96" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C96" s="13">
         <v>4</v>
@@ -14044,7 +14046,7 @@
         <v>36</v>
       </c>
       <c r="F96" s="58" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="G96"/>
       <c r="H96"/>
@@ -15070,7 +15072,7 @@
         <v>32</v>
       </c>
       <c r="B97" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C97" s="13">
         <v>4</v>
@@ -15082,7 +15084,7 @@
         <v>37</v>
       </c>
       <c r="F97" s="58" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="G97"/>
       <c r="H97"/>
@@ -16108,7 +16110,7 @@
         <v>32</v>
       </c>
       <c r="B98" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C98" s="13">
         <v>4</v>
@@ -16120,7 +16122,7 @@
         <v>38</v>
       </c>
       <c r="F98" s="58" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="G98"/>
       <c r="H98"/>
@@ -17146,7 +17148,7 @@
         <v>32</v>
       </c>
       <c r="B99" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C99" s="13">
         <v>4</v>
@@ -17158,7 +17160,7 @@
         <v>39</v>
       </c>
       <c r="F99" s="58" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="G99"/>
       <c r="H99"/>
@@ -18184,7 +18186,7 @@
         <v>32</v>
       </c>
       <c r="B100" s="17" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C100" s="17">
         <v>4</v>
@@ -18196,7 +18198,7 @@
         <v>40</v>
       </c>
       <c r="F100" s="58" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="K100" s="13"/>
     </row>
@@ -18214,13 +18216,13 @@
         <v>120</v>
       </c>
       <c r="B102" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C102" s="13">
         <v>4</v>
       </c>
       <c r="D102" s="22" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="E102" s="16" t="s">
         <v>121</v>
@@ -18235,13 +18237,13 @@
         <v>120</v>
       </c>
       <c r="B103" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C103" s="13">
         <v>4</v>
       </c>
       <c r="D103" s="22" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="E103" s="16" t="s">
         <v>122</v>
@@ -18256,13 +18258,13 @@
         <v>120</v>
       </c>
       <c r="B104" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C104" s="13">
         <v>4</v>
       </c>
       <c r="D104" s="22" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="E104" s="16" t="s">
         <v>123</v>
@@ -18277,13 +18279,13 @@
         <v>120</v>
       </c>
       <c r="B105" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C105" s="13">
         <v>4</v>
       </c>
       <c r="D105" s="22" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="E105" s="16" t="s">
         <v>124</v>
@@ -18298,13 +18300,13 @@
         <v>120</v>
       </c>
       <c r="B106" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C106" s="13">
         <v>4</v>
       </c>
       <c r="D106" s="22" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="E106" s="16" t="s">
         <v>23</v>
@@ -18313,7 +18315,7 @@
         <v>19706</v>
       </c>
       <c r="G106" s="24" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
     </row>
     <row r="107" spans="1:1024" x14ac:dyDescent="0.25">
@@ -18321,13 +18323,13 @@
         <v>120</v>
       </c>
       <c r="B107" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C107" s="13">
         <v>4</v>
       </c>
       <c r="D107" s="22" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="E107" s="16" t="s">
         <v>125</v>
@@ -18336,7 +18338,7 @@
         <v>34</v>
       </c>
       <c r="G107" s="25" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
     </row>
     <row r="108" spans="1:1024" x14ac:dyDescent="0.25">
@@ -18344,13 +18346,13 @@
         <v>120</v>
       </c>
       <c r="B108" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C108" s="13">
         <v>4</v>
       </c>
       <c r="D108" s="22" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="E108" s="16" t="s">
         <v>25</v>
@@ -18365,13 +18367,13 @@
         <v>120</v>
       </c>
       <c r="B109" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C109" s="13">
         <v>4</v>
       </c>
       <c r="D109" s="22" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="E109" s="16" t="s">
         <v>126</v>
@@ -18395,13 +18397,13 @@
         <v>22</v>
       </c>
       <c r="B111" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C111" s="13">
         <v>4</v>
       </c>
       <c r="D111" s="22" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="E111" s="16" t="s">
         <v>23</v>
@@ -19432,13 +19434,13 @@
         <v>22</v>
       </c>
       <c r="B112" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C112" s="13">
         <v>4</v>
       </c>
       <c r="D112" s="22" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="E112" s="16" t="s">
         <v>24</v>
@@ -20469,13 +20471,13 @@
         <v>22</v>
       </c>
       <c r="B113" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C113" s="13">
         <v>4</v>
       </c>
       <c r="D113" s="22" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="E113" s="16" t="s">
         <v>25</v>
@@ -21506,13 +21508,13 @@
         <v>22</v>
       </c>
       <c r="B114" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C114" s="13">
         <v>4</v>
       </c>
       <c r="D114" s="22" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="E114" s="16" t="s">
         <v>26</v>
@@ -22543,13 +22545,13 @@
         <v>22</v>
       </c>
       <c r="B115" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C115" s="13">
         <v>4</v>
       </c>
       <c r="D115" s="22" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="E115" s="16" t="s">
         <v>27</v>
@@ -23580,13 +23582,13 @@
         <v>22</v>
       </c>
       <c r="B116" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C116" s="13">
         <v>4</v>
       </c>
       <c r="D116" s="22" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="E116" s="16" t="s">
         <v>28</v>
@@ -24617,13 +24619,13 @@
         <v>22</v>
       </c>
       <c r="B117" s="43" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C117" s="43">
         <v>4</v>
       </c>
       <c r="D117" s="43" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="E117" s="43" t="s">
         <v>29</v>
@@ -24632,7 +24634,7 @@
         <v>35</v>
       </c>
       <c r="G117" s="32" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="H117"/>
       <c r="I117"/>
@@ -26681,7 +26683,7 @@
         <v>90</v>
       </c>
       <c r="B119" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C119" s="13">
         <v>4</v>
@@ -26693,7 +26695,7 @@
         <v>91</v>
       </c>
       <c r="F119" s="42" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="G119"/>
     </row>
@@ -26702,7 +26704,7 @@
         <v>90</v>
       </c>
       <c r="B120" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C120" s="13">
         <v>4</v>
@@ -26714,7 +26716,7 @@
         <v>92</v>
       </c>
       <c r="F120" s="42" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="G120"/>
     </row>
@@ -26723,7 +26725,7 @@
         <v>90</v>
       </c>
       <c r="B121" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C121" s="13">
         <v>4</v>
@@ -26735,7 +26737,7 @@
         <v>93</v>
       </c>
       <c r="F121" s="42" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="G121"/>
     </row>
@@ -26753,7 +26755,7 @@
         <v>21</v>
       </c>
       <c r="B123" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C123" s="13">
         <v>4</v>
@@ -27791,7 +27793,7 @@
         <v>21</v>
       </c>
       <c r="B124" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C124" s="13">
         <v>4</v>
@@ -29854,7 +29856,7 @@
         <v>94</v>
       </c>
       <c r="H126" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="I126" s="13">
         <v>4</v>
@@ -29869,7 +29871,7 @@
         <v>25000</v>
       </c>
       <c r="M126" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
     </row>
     <row r="127" spans="1:1024" x14ac:dyDescent="0.25">
@@ -29877,7 +29879,7 @@
         <v>94</v>
       </c>
       <c r="H127" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="I127" s="13">
         <v>4</v>
@@ -29898,7 +29900,7 @@
         <v>94</v>
       </c>
       <c r="H128" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="I128" s="13">
         <v>4</v>
@@ -29919,7 +29921,7 @@
         <v>94</v>
       </c>
       <c r="H129" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="I129" s="13">
         <v>4</v>
@@ -29940,7 +29942,7 @@
         <v>94</v>
       </c>
       <c r="H130" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="I130" s="13">
         <v>4</v>
@@ -29961,7 +29963,7 @@
         <v>94</v>
       </c>
       <c r="H131" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="I131" s="13">
         <v>4</v>
@@ -29982,7 +29984,7 @@
         <v>94</v>
       </c>
       <c r="H132" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="I132" s="13">
         <v>4</v>
@@ -30018,16 +30020,16 @@
         <v>17</v>
       </c>
       <c r="H134" s="32" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="I134" s="32" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="J134" s="32">
         <v>4</v>
       </c>
       <c r="K134" s="31" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="M134" s="32"/>
       <c r="N134" s="16"/>
@@ -32074,13 +32076,13 @@
         <v>78</v>
       </c>
       <c r="H136" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="I136" s="13">
         <v>4</v>
       </c>
       <c r="J136" s="22" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="K136" s="16" t="s">
         <v>19</v>
@@ -32094,13 +32096,13 @@
         <v>78</v>
       </c>
       <c r="H137" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="I137" s="13">
         <v>4</v>
       </c>
       <c r="J137" s="22" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="K137" s="16" t="s">
         <v>20</v>
@@ -32114,13 +32116,13 @@
         <v>78</v>
       </c>
       <c r="H138" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="I138" s="13">
         <v>4</v>
       </c>
       <c r="J138" s="22" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="K138" s="16" t="s">
         <v>56</v>
@@ -32134,13 +32136,13 @@
         <v>78</v>
       </c>
       <c r="H139" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="I139" s="13">
         <v>4</v>
       </c>
       <c r="J139" s="22" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="K139" s="16" t="s">
         <v>57</v>
@@ -32154,13 +32156,13 @@
         <v>78</v>
       </c>
       <c r="H140" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="I140" s="13">
         <v>4</v>
       </c>
       <c r="J140" s="22" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="K140" s="16" t="s">
         <v>58</v>
@@ -32174,13 +32176,13 @@
         <v>78</v>
       </c>
       <c r="H141" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="I141" s="13">
         <v>4</v>
       </c>
       <c r="J141" s="22" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="K141" s="16" t="s">
         <v>59</v>
@@ -32194,13 +32196,13 @@
         <v>78</v>
       </c>
       <c r="H142" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="I142" s="13">
         <v>4</v>
       </c>
       <c r="J142" s="22" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="K142" s="16" t="s">
         <v>60</v>
@@ -32214,13 +32216,13 @@
         <v>78</v>
       </c>
       <c r="H143" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="I143" s="13">
         <v>4</v>
       </c>
       <c r="J143" s="22" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="K143" s="16" t="s">
         <v>61</v>
@@ -32234,13 +32236,13 @@
         <v>78</v>
       </c>
       <c r="H144" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="I144" s="13">
         <v>4</v>
       </c>
       <c r="J144" s="22" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="K144" s="16" t="s">
         <v>62</v>
@@ -32254,13 +32256,13 @@
         <v>78</v>
       </c>
       <c r="H145" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="I145" s="13">
         <v>4</v>
       </c>
       <c r="J145" s="22" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="K145" s="16" t="s">
         <v>63</v>
@@ -32274,13 +32276,13 @@
         <v>78</v>
       </c>
       <c r="H146" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="I146" s="13">
         <v>4</v>
       </c>
       <c r="J146" s="22" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="K146" s="16" t="s">
         <v>64</v>
@@ -32294,13 +32296,13 @@
         <v>78</v>
       </c>
       <c r="H147" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="I147" s="13">
         <v>4</v>
       </c>
       <c r="J147" s="22" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="K147" s="16" t="s">
         <v>65</v>
@@ -32314,13 +32316,13 @@
         <v>78</v>
       </c>
       <c r="H148" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="I148" s="13">
         <v>4</v>
       </c>
       <c r="J148" s="22" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="K148" s="16" t="s">
         <v>66</v>
@@ -32334,13 +32336,13 @@
         <v>78</v>
       </c>
       <c r="H149" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="I149" s="13">
         <v>4</v>
       </c>
       <c r="J149" s="22" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="K149" s="16" t="s">
         <v>67</v>
@@ -32354,13 +32356,13 @@
         <v>78</v>
       </c>
       <c r="H150" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="I150" s="13">
         <v>4</v>
       </c>
       <c r="J150" s="22" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="K150" s="16" t="s">
         <v>68</v>
@@ -32374,13 +32376,13 @@
         <v>78</v>
       </c>
       <c r="H151" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="I151" s="13">
         <v>4</v>
       </c>
       <c r="J151" s="22" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="K151" s="16" t="s">
         <v>69</v>
@@ -32394,13 +32396,13 @@
         <v>78</v>
       </c>
       <c r="H152" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="I152" s="13">
         <v>4</v>
       </c>
       <c r="J152" s="22" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="K152" s="16" t="s">
         <v>70</v>
@@ -32414,13 +32416,13 @@
         <v>78</v>
       </c>
       <c r="H153" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="I153" s="13">
         <v>4</v>
       </c>
       <c r="J153" s="22" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="K153" s="16" t="s">
         <v>71</v>
@@ -32434,13 +32436,13 @@
         <v>78</v>
       </c>
       <c r="H154" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="I154" s="13">
         <v>4</v>
       </c>
       <c r="J154" s="22" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="K154" s="16" t="s">
         <v>72</v>
@@ -32454,13 +32456,13 @@
         <v>78</v>
       </c>
       <c r="H155" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="I155" s="13">
         <v>4</v>
       </c>
       <c r="J155" s="22" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="K155" s="16" t="s">
         <v>73</v>
@@ -32474,13 +32476,13 @@
         <v>78</v>
       </c>
       <c r="H156" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="I156" s="13">
         <v>4</v>
       </c>
       <c r="J156" s="22" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="K156" s="16" t="s">
         <v>74</v>
@@ -32494,13 +32496,13 @@
         <v>78</v>
       </c>
       <c r="H157" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="I157" s="13">
         <v>4</v>
       </c>
       <c r="J157" s="22" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="K157" s="16" t="s">
         <v>75</v>
@@ -32514,13 +32516,13 @@
         <v>78</v>
       </c>
       <c r="H158" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="I158" s="13">
         <v>4</v>
       </c>
       <c r="J158" s="22" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="K158" s="16" t="s">
         <v>76</v>
@@ -32534,13 +32536,13 @@
         <v>78</v>
       </c>
       <c r="H159" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="I159" s="13">
         <v>4</v>
       </c>
       <c r="J159" s="22" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="K159" s="16" t="s">
         <v>77</v>
@@ -32563,7 +32565,7 @@
         <v>81</v>
       </c>
       <c r="B161" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C161" s="13">
         <v>4</v>
@@ -32584,7 +32586,7 @@
         <v>81</v>
       </c>
       <c r="B162" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C162" s="13">
         <v>4</v>
@@ -32605,7 +32607,7 @@
         <v>81</v>
       </c>
       <c r="B163" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C163" s="13">
         <v>4</v>
@@ -32617,7 +32619,7 @@
         <v>80</v>
       </c>
       <c r="F163" s="39" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="G163"/>
     </row>
@@ -32626,7 +32628,7 @@
         <v>81</v>
       </c>
       <c r="B164" s="16" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C164" s="16">
         <v>4</v>
@@ -32635,13 +32637,13 @@
         <v>485</v>
       </c>
       <c r="E164" s="32" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="F164" s="33" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="G164" s="32" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="H164" s="16"/>
       <c r="I164" s="16"/>
@@ -33678,10 +33680,10 @@
         <v>41</v>
       </c>
       <c r="I166" s="16" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="K166" s="21" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="L166" s="16" t="s">
         <v>33</v>
@@ -33695,7 +33697,7 @@
         <v>41</v>
       </c>
       <c r="I167" s="16" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="K167" s="21"/>
       <c r="L167" s="16" t="s">
@@ -33710,7 +33712,7 @@
         <v>41</v>
       </c>
       <c r="I168" s="16" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="K168" s="21"/>
       <c r="L168" s="16" t="s">
@@ -33725,7 +33727,7 @@
         <v>41</v>
       </c>
       <c r="I169" s="16" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="J169" s="16">
         <v>4</v>
@@ -33743,7 +33745,7 @@
         <v>41</v>
       </c>
       <c r="I170" s="16" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="J170" s="16">
         <v>4</v>
@@ -33761,7 +33763,7 @@
         <v>41</v>
       </c>
       <c r="I171" s="16" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="J171" s="16">
         <v>4</v>
@@ -33779,7 +33781,7 @@
         <v>41</v>
       </c>
       <c r="I172" s="16" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="J172" s="16">
         <v>4</v>
@@ -33797,7 +33799,7 @@
         <v>41</v>
       </c>
       <c r="I173" s="16" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="J173" s="16">
         <v>4</v>
@@ -33821,13 +33823,13 @@
         <v>127</v>
       </c>
       <c r="B175" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C175" s="13">
         <v>4</v>
       </c>
       <c r="D175" s="47" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="E175" s="16" t="s">
         <v>121</v>
@@ -33842,13 +33844,13 @@
         <v>127</v>
       </c>
       <c r="B176" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C176" s="13">
         <v>4</v>
       </c>
       <c r="D176" s="47" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="E176" s="16" t="s">
         <v>122</v>
@@ -33863,13 +33865,13 @@
         <v>127</v>
       </c>
       <c r="B177" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C177" s="13">
         <v>4</v>
       </c>
       <c r="D177" s="47" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="E177" s="16" t="s">
         <v>123</v>
@@ -33884,13 +33886,13 @@
         <v>127</v>
       </c>
       <c r="B178" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C178" s="13">
         <v>4</v>
       </c>
       <c r="D178" s="47" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="E178" s="16" t="s">
         <v>124</v>
@@ -33905,13 +33907,13 @@
         <v>127</v>
       </c>
       <c r="B179" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C179" s="13">
         <v>4</v>
       </c>
       <c r="D179" s="47" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="E179" s="16" t="s">
         <v>23</v>
@@ -33920,7 +33922,7 @@
         <v>19706</v>
       </c>
       <c r="G179" s="24" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
     </row>
     <row r="180" spans="1:1025" x14ac:dyDescent="0.25">
@@ -33928,13 +33930,13 @@
         <v>127</v>
       </c>
       <c r="B180" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C180" s="13">
         <v>4</v>
       </c>
       <c r="D180" s="47" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="E180" s="16" t="s">
         <v>125</v>
@@ -33943,7 +33945,7 @@
         <v>34</v>
       </c>
       <c r="G180" s="25" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
     </row>
     <row r="181" spans="1:1025" x14ac:dyDescent="0.25">
@@ -33951,13 +33953,13 @@
         <v>127</v>
       </c>
       <c r="B181" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C181" s="13">
         <v>4</v>
       </c>
       <c r="D181" s="47" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="E181" s="16" t="s">
         <v>25</v>
@@ -33972,13 +33974,13 @@
         <v>127</v>
       </c>
       <c r="B182" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C182" s="13">
         <v>4</v>
       </c>
       <c r="D182" s="47" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="E182" s="16" t="s">
         <v>126</v>
@@ -34004,13 +34006,13 @@
         <v>31</v>
       </c>
       <c r="I184" s="16" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="J184" s="16">
         <v>4</v>
       </c>
       <c r="K184" s="21" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="L184" s="16" t="s">
         <v>23</v>
@@ -35038,7 +35040,7 @@
         <v>31</v>
       </c>
       <c r="I185" s="16" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="J185" s="16">
         <v>4</v>
@@ -36070,7 +36072,7 @@
         <v>31</v>
       </c>
       <c r="I186" s="16" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="J186" s="16">
         <v>4</v>
@@ -37102,7 +37104,7 @@
         <v>31</v>
       </c>
       <c r="I187" s="16" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="J187" s="16">
         <v>4</v>
@@ -38135,7 +38137,7 @@
         <v>31</v>
       </c>
       <c r="I188" s="16" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="J188" s="16">
         <v>4</v>
@@ -39168,7 +39170,7 @@
         <v>31</v>
       </c>
       <c r="I189" s="16" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="J189" s="16">
         <v>4</v>
@@ -40200,13 +40202,13 @@
       <c r="E190" s="43"/>
       <c r="F190" s="45"/>
       <c r="G190" s="32" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="H190" s="43" t="s">
         <v>31</v>
       </c>
       <c r="I190" s="43" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="J190" s="43">
         <v>4</v>
@@ -41251,13 +41253,13 @@
         <v>101</v>
       </c>
       <c r="B192" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C192" s="13">
         <v>4</v>
       </c>
       <c r="D192" s="22" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="E192" s="16" t="s">
         <v>102</v>
@@ -41266,7 +41268,7 @@
         <v>601.76969999999994</v>
       </c>
       <c r="G192" s="48" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
     </row>
     <row r="193" spans="1:7" x14ac:dyDescent="0.25">
@@ -41274,13 +41276,13 @@
         <v>101</v>
       </c>
       <c r="B193" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C193" s="13">
         <v>4</v>
       </c>
       <c r="D193" s="22" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="E193" s="16" t="s">
         <v>103</v>
@@ -41289,7 +41291,7 @@
         <v>4.9606469999999998</v>
       </c>
       <c r="G193" s="48" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
     </row>
     <row r="194" spans="1:7" x14ac:dyDescent="0.25">
@@ -41297,13 +41299,13 @@
         <v>101</v>
       </c>
       <c r="B194" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C194" s="13">
         <v>4</v>
       </c>
       <c r="D194" s="22" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="E194" s="16" t="s">
         <v>104</v>
@@ -41318,13 +41320,13 @@
         <v>101</v>
       </c>
       <c r="B195" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C195" s="13">
         <v>4</v>
       </c>
       <c r="D195" s="22" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="E195" s="16" t="s">
         <v>105</v>
@@ -41339,13 +41341,13 @@
         <v>101</v>
       </c>
       <c r="B196" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C196" s="13">
         <v>4</v>
       </c>
       <c r="D196" s="22" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="E196" s="16" t="s">
         <v>106</v>
@@ -41360,13 +41362,13 @@
         <v>101</v>
       </c>
       <c r="B197" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C197" s="13">
         <v>4</v>
       </c>
       <c r="D197" s="22" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="E197" s="16" t="s">
         <v>107</v>
@@ -41383,13 +41385,13 @@
         <v>101</v>
       </c>
       <c r="B198" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C198" s="13">
         <v>4</v>
       </c>
       <c r="D198" s="22" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="E198" s="16" t="s">
         <v>108</v>
@@ -41398,7 +41400,7 @@
         <v>-0.15820000000000001</v>
       </c>
       <c r="G198" s="30" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
     </row>
     <row r="199" spans="1:7" x14ac:dyDescent="0.25">
@@ -41406,13 +41408,13 @@
         <v>101</v>
       </c>
       <c r="B199" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C199" s="13">
         <v>4</v>
       </c>
       <c r="D199" s="22" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="E199" s="16" t="s">
         <v>109</v>
@@ -41429,13 +41431,13 @@
         <v>101</v>
       </c>
       <c r="B200" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C200" s="13">
         <v>4</v>
       </c>
       <c r="D200" s="22" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="E200" s="16" t="s">
         <v>110</v>
@@ -41450,13 +41452,13 @@
         <v>101</v>
       </c>
       <c r="B201" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C201" s="13">
         <v>4</v>
       </c>
       <c r="D201" s="22" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="E201" s="16" t="s">
         <v>111</v>
@@ -41471,13 +41473,13 @@
         <v>101</v>
       </c>
       <c r="B202" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C202" s="13">
         <v>4</v>
       </c>
       <c r="D202" s="22" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="E202" s="16" t="s">
         <v>112</v>
@@ -41492,13 +41494,13 @@
         <v>101</v>
       </c>
       <c r="B203" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C203" s="13">
         <v>4</v>
       </c>
       <c r="D203" s="22" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="E203" s="16" t="s">
         <v>113</v>
@@ -41513,13 +41515,13 @@
         <v>101</v>
       </c>
       <c r="B204" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C204" s="13">
         <v>4</v>
       </c>
       <c r="D204" s="22" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="E204" s="16" t="s">
         <v>114</v>
@@ -41534,13 +41536,13 @@
         <v>101</v>
       </c>
       <c r="B205" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C205" s="13">
         <v>4</v>
       </c>
       <c r="D205" s="22" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="E205" s="16" t="s">
         <v>115</v>
@@ -41555,13 +41557,13 @@
         <v>101</v>
       </c>
       <c r="B206" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C206" s="13">
         <v>4</v>
       </c>
       <c r="D206" s="22" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="E206" s="16" t="s">
         <v>116</v>
@@ -41576,13 +41578,13 @@
         <v>101</v>
       </c>
       <c r="B207" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C207" s="13">
         <v>4</v>
       </c>
       <c r="D207" s="22" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="E207" s="16" t="s">
         <v>117</v>
@@ -41597,13 +41599,13 @@
         <v>101</v>
       </c>
       <c r="B208" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C208" s="13">
         <v>4</v>
       </c>
       <c r="D208" s="22" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="E208" s="16" t="s">
         <v>118</v>
@@ -41618,13 +41620,13 @@
         <v>101</v>
       </c>
       <c r="B209" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C209" s="13">
         <v>4</v>
       </c>
       <c r="D209" s="22" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="E209" s="16" t="s">
         <v>119</v>
@@ -41648,7 +41650,7 @@
         <v>100</v>
       </c>
       <c r="B211" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C211" s="13">
         <v>4</v>
@@ -41669,7 +41671,7 @@
         <v>100</v>
       </c>
       <c r="B212" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C212" s="13">
         <v>4</v>
@@ -41696,10 +41698,10 @@
     </row>
     <row r="214" spans="1:1025" x14ac:dyDescent="0.25">
       <c r="A214" s="32" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="B214" s="28" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C214" s="28">
         <v>4</v>
@@ -42765,13 +42767,13 @@
         <v>128</v>
       </c>
       <c r="B219" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C219" s="13">
         <v>4</v>
       </c>
       <c r="D219" s="19" t="s">
-        <v>129</v>
+        <v>179</v>
       </c>
       <c r="E219" s="16"/>
       <c r="G219" s="13" t="s">
@@ -42779,35 +42781,36 @@
       </c>
     </row>
     <row r="220" spans="1:1025" x14ac:dyDescent="0.25">
-      <c r="A220" s="13" t="s">
-        <v>130</v>
-      </c>
-      <c r="B220" s="13" t="s">
-        <v>142</v>
-      </c>
-      <c r="C220" s="13">
+      <c r="H220" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="I220" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="J220" s="13">
         <v>4</v>
       </c>
-      <c r="D220" s="19" t="s">
-        <v>131</v>
-      </c>
-      <c r="E220" s="16"/>
-      <c r="G220" s="13" t="s">
+      <c r="K220" s="19" t="s">
+        <v>179</v>
+      </c>
+      <c r="L220" s="16"/>
+      <c r="M220" s="37"/>
+      <c r="N220" s="13" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="221" spans="1:1025" x14ac:dyDescent="0.25">
       <c r="A221" s="13" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B221" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C221" s="13">
         <v>4</v>
       </c>
       <c r="D221" s="19" t="s">
-        <v>133</v>
+        <v>180</v>
       </c>
       <c r="E221" s="16"/>
       <c r="G221" s="13" t="s">
@@ -42824,16 +42827,16 @@
     </row>
     <row r="223" spans="1:1025" x14ac:dyDescent="0.25">
       <c r="A223" s="13" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B223" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C223" s="13">
         <v>4</v>
       </c>
       <c r="D223" s="19" t="s">
-        <v>135</v>
+        <v>181</v>
       </c>
       <c r="E223" s="16"/>
       <c r="G223" s="13" t="s">
@@ -42842,16 +42845,16 @@
     </row>
     <row r="224" spans="1:1025" x14ac:dyDescent="0.25">
       <c r="A224" s="13" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="B224" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C224" s="13">
         <v>4</v>
       </c>
       <c r="D224" s="19" t="s">
-        <v>137</v>
+        <v>182</v>
       </c>
       <c r="E224" s="16"/>
       <c r="G224" s="13" t="s">
@@ -42860,16 +42863,16 @@
     </row>
     <row r="225" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A225" s="13" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="B225" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C225" s="13">
         <v>4</v>
       </c>
       <c r="D225" s="19" t="s">
-        <v>139</v>
+        <v>183</v>
       </c>
       <c r="G225" s="13" t="s">
         <v>17</v>
@@ -42877,16 +42880,16 @@
     </row>
     <row r="226" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A226" s="13" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="B226" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C226" s="13">
         <v>4</v>
       </c>
       <c r="D226" s="19" t="s">
-        <v>141</v>
+        <v>184</v>
       </c>
       <c r="G226" s="13" t="s">
         <v>17</v>

</xml_diff>